<commit_message>
Cambiamos el LDR por un sensor infrarojo
</commit_message>
<xml_diff>
--- a/Presupuesto.xlsx
+++ b/Presupuesto.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t xml:space="preserve">LISTA DE ELEMENTOS</t>
   </si>
@@ -34,7 +34,7 @@
     <t xml:space="preserve">Precio</t>
   </si>
   <si>
-    <t xml:space="preserve">LDR</t>
+    <t xml:space="preserve"> INFRAROGO</t>
   </si>
   <si>
     <t xml:space="preserve">POTES </t>
@@ -53,6 +53,9 @@
   </si>
   <si>
     <t xml:space="preserve">LED</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  </t>
   </si>
   <si>
     <t xml:space="preserve">Total</t>
@@ -65,17 +68,17 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="[$€-410]\ #,##0.00;[RED]\-[$€-410]\ #,##0.00"/>
     <numFmt numFmtId="166" formatCode="[$$-2C0A]#,##0.00;[RED]\([$$-2C0A]#,##0.00\)"/>
-    <numFmt numFmtId="167" formatCode="[$$-2C0A]#,##0.00;[RED]\([$$-2C0A]#,##0.00\)"/>
   </numFmts>
   <fonts count="8">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -98,24 +101,28 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <i val="true"/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="6">
@@ -183,9 +190,11 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -234,7 +243,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -242,11 +251,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="20" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -331,15 +336,16 @@
   <dimension ref="B2:H15"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
+      <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.49"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="5.26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="5.27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="17.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="132.39"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -369,8 +375,7 @@
         <v>2</v>
       </c>
       <c r="D5" s="8" t="n">
-        <f aca="false">25*C5</f>
-        <v>50</v>
+        <v>400</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -447,32 +452,35 @@
       <c r="E11" s="8"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B12" s="0" t="s">
+        <v>11</v>
+      </c>
       <c r="D12" s="8"/>
       <c r="E12" s="8"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="10" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C13" s="11"/>
       <c r="D13" s="12" t="n">
         <f aca="false">SUM(D5:D12)</f>
-        <v>5190</v>
+        <v>5540</v>
       </c>
       <c r="E13" s="8"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="D14" s="14" t="n">
+        <v>13</v>
+      </c>
+      <c r="D14" s="8" t="n">
         <f aca="false">D13/4</f>
-        <v>1297.5</v>
+        <v>1385</v>
       </c>
       <c r="E14" s="8"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D15" s="15"/>
+      <c r="D15" s="14"/>
       <c r="E15" s="8"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Agregado mas cosas al presupuesto
</commit_message>
<xml_diff>
--- a/Presupuesto.xlsx
+++ b/Presupuesto.xlsx
@@ -10,6 +10,13 @@
   <sheets>
     <sheet name="Hoja1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName function="false" hidden="false" name="E10000000000" vbProcedure="false">Hoja1!$E$1</definedName>
+    <definedName function="false" hidden="false" name="E100000000000" vbProcedure="false">Hoja1!$E$1</definedName>
+    <definedName function="false" hidden="false" name="E100000000000000000000" vbProcedure="false">Hoja1!$E$1</definedName>
+    <definedName function="false" hidden="false" name="E1000000000000000000000000000000" vbProcedure="false">Hoja1!$E$1</definedName>
+    <definedName function="false" hidden="false" name="E100000000010" vbProcedure="false">Hoja1!$E$1</definedName>
+  </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
@@ -20,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t xml:space="preserve">LISTA DE ELEMENTOS</t>
   </si>
@@ -31,7 +38,10 @@
     <t xml:space="preserve">Cant.</t>
   </si>
   <si>
-    <t xml:space="preserve">Precio</t>
+    <t xml:space="preserve">Precio Unitario</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Precio Total</t>
   </si>
   <si>
     <t xml:space="preserve">BUZZER</t>
@@ -43,22 +53,43 @@
     <t xml:space="preserve">SENS COLOR</t>
   </si>
   <si>
-    <t xml:space="preserve">X</t>
-  </si>
-  <si>
     <t xml:space="preserve">INFRAROJO</t>
   </si>
   <si>
-    <t xml:space="preserve">SENS CAPAC</t>
+    <t xml:space="preserve">SENS CAPACI</t>
   </si>
   <si>
     <t xml:space="preserve">BATERIA</t>
   </si>
   <si>
-    <t xml:space="preserve">MOTOR SP6</t>
+    <t xml:space="preserve">MOTOR </t>
   </si>
   <si>
     <t xml:space="preserve">BLUETOOTH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BEBEDERO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BOTELLA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PLATITO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STEPDOWN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MADERAS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PLACAS TEC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">COMPS.GENE</t>
   </si>
   <si>
     <t xml:space="preserve">Total</t>
@@ -71,10 +102,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="[$€-410]\ #,##0.00;[RED]\-[$€-410]\ #,##0.00"/>
     <numFmt numFmtId="166" formatCode="[$$-2C0A]#,##0.00;[RED]\([$$-2C0A]#,##0.00\)"/>
+    <numFmt numFmtId="167" formatCode="[$$-2C0A]#,##0.00;[RED]\([$$-2C0A]#,##0.00\)"/>
   </numFmts>
   <fonts count="7">
     <font>
@@ -198,15 +230,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -222,6 +250,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -230,7 +262,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="167" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -315,19 +347,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B2:H15"/>
+  <dimension ref="B2:H779"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D13" activeCellId="0" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.49"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="5.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="17.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="132.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="16.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="14.29"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -336,67 +368,93 @@
         <v>0</v>
       </c>
       <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D4" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H4" s="7"/>
+      <c r="E4" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="H4" s="6"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="0" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C5" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="D5" s="8"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7" t="n">
+        <f aca="false">D5*C5</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C6" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="D6" s="9"/>
-      <c r="E6" s="8"/>
+        <v>3</v>
+      </c>
+      <c r="D6" s="8"/>
+      <c r="E6" s="7" t="n">
+        <f aca="false">D6*C6</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
+      <c r="C7" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D7" s="7" t="n">
+        <v>1029</v>
+      </c>
+      <c r="E7" s="7" t="n">
+        <f aca="false">D7*C7</f>
+        <v>1029</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
+      <c r="C8" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="D8" s="7" t="n">
+        <v>606.25</v>
+      </c>
+      <c r="E8" s="7" t="n">
+        <f aca="false">D8*C8</f>
+        <v>1818.75</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
+      <c r="C9" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="D9" s="7" t="n">
+        <v>483.11</v>
+      </c>
+      <c r="E9" s="7" t="n">
+        <f aca="false">D9*C9</f>
+        <v>1449.33</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="0" t="s">
@@ -405,8 +463,13 @@
       <c r="C10" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
+      <c r="D10" s="7" t="n">
+        <v>1879.4</v>
+      </c>
+      <c r="E10" s="7" t="n">
+        <f aca="false">C10*D10</f>
+        <v>1879.4</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="0" t="s">
@@ -415,8 +478,13 @@
       <c r="C11" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="D11" s="8"/>
-      <c r="E11" s="8"/>
+      <c r="D11" s="7" t="n">
+        <v>1900</v>
+      </c>
+      <c r="E11" s="7" t="n">
+        <f aca="false">D11*C11</f>
+        <v>1900</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="0" t="s">
@@ -425,32 +493,114 @@
       <c r="C12" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="D12" s="8"/>
-      <c r="E12" s="8"/>
+      <c r="D12" s="7" t="n">
+        <v>650</v>
+      </c>
+      <c r="E12" s="7" t="n">
+        <f aca="false">D12*C12</f>
+        <v>650</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E13" s="8"/>
+      <c r="B13" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D13" s="9" t="n">
+        <v>1600</v>
+      </c>
+      <c r="E13" s="9" t="n">
+        <f aca="false">D13*C13</f>
+        <v>1600</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="C14" s="11"/>
-      <c r="D14" s="12" t="n">
-        <f aca="false">SUM(D5:D12)</f>
+      <c r="B14" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D14" s="9"/>
+      <c r="E14" s="9"/>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B15" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9"/>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B16" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="C16" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D16" s="9"/>
+      <c r="E16" s="9"/>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B17" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="C17" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D17" s="9"/>
+      <c r="E17" s="9"/>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B18" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="D18" s="9"/>
+      <c r="E18" s="9"/>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B19" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="D19" s="9"/>
+      <c r="E19" s="9"/>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B20" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="D20" s="9"/>
+      <c r="E20" s="9"/>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B24" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C24" s="11"/>
+      <c r="D24" s="11"/>
+      <c r="E24" s="12" t="n">
+        <f aca="false">SUM(E5:E13)</f>
+        <v>10326.48</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B25" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="E25" s="7" t="n">
+        <f aca="false">E24/4</f>
+        <v>2581.62</v>
+      </c>
+    </row>
+    <row r="779" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E779" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="E14" s="8"/>
-    </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="D15" s="8" t="n">
-        <f aca="false">D14/4</f>
-        <v>0</v>
-      </c>
-      <c r="E15" s="8"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
Diseño final de plaqueta terminado
</commit_message>
<xml_diff>
--- a/Presupuesto.xlsx
+++ b/Presupuesto.xlsx
@@ -102,11 +102,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="[$€-410]\ #,##0.00;[RED]\-[$€-410]\ #,##0.00"/>
     <numFmt numFmtId="166" formatCode="[$$-2C0A]#,##0.00;[RED]\([$$-2C0A]#,##0.00\)"/>
-    <numFmt numFmtId="167" formatCode="[$$-2C0A]#,##0.00;[RED]\([$$-2C0A]#,##0.00\)"/>
   </numFmts>
   <fonts count="7">
     <font>
@@ -213,7 +212,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -250,10 +249,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -262,7 +257,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -350,10 +345,10 @@
   <dimension ref="B2:H779"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D13" activeCellId="0" sqref="D13"/>
+      <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.49"/>
@@ -508,10 +503,10 @@
       <c r="C13" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="D13" s="9" t="n">
+      <c r="D13" s="7" t="n">
         <v>1600</v>
       </c>
-      <c r="E13" s="9" t="n">
+      <c r="E13" s="7" t="n">
         <f aca="false">D13*C13</f>
         <v>1600</v>
       </c>
@@ -523,8 +518,11 @@
       <c r="C14" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="D14" s="9"/>
-      <c r="E14" s="9"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="7" t="n">
+        <f aca="false">D14*C14</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="0" t="s">
@@ -533,8 +531,11 @@
       <c r="C15" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="D15" s="9"/>
-      <c r="E15" s="9"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7" t="n">
+        <f aca="false">D15*C15</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="0" t="s">
@@ -543,8 +544,13 @@
       <c r="C16" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="D16" s="9"/>
-      <c r="E16" s="9"/>
+      <c r="D16" s="7" t="n">
+        <v>139</v>
+      </c>
+      <c r="E16" s="7" t="n">
+        <f aca="false">D16*C16</f>
+        <v>139</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="0" t="s">
@@ -553,48 +559,63 @@
       <c r="C17" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="D17" s="9"/>
-      <c r="E17" s="9"/>
+      <c r="D17" s="7" t="n">
+        <v>839</v>
+      </c>
+      <c r="E17" s="7" t="n">
+        <f aca="false">D17*C17</f>
+        <v>839</v>
+      </c>
+      <c r="F17" s="7"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="D18" s="9"/>
-      <c r="E18" s="9"/>
+      <c r="D18" s="7"/>
+      <c r="E18" s="7" t="n">
+        <f aca="false">D18*C18</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="D19" s="9"/>
-      <c r="E19" s="9"/>
+      <c r="D19" s="7"/>
+      <c r="E19" s="7" t="n">
+        <f aca="false">D19*C19</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="D20" s="9"/>
-      <c r="E20" s="9"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="7" t="n">
+        <f aca="false">D20*C20</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B24" s="10" t="s">
+      <c r="B24" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="C24" s="11"/>
-      <c r="D24" s="11"/>
-      <c r="E24" s="12" t="n">
-        <f aca="false">SUM(E5:E13)</f>
-        <v>10326.48</v>
+      <c r="C24" s="10"/>
+      <c r="D24" s="10"/>
+      <c r="E24" s="11" t="n">
+        <f aca="false">SUM(E5:E20)</f>
+        <v>11304.48</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="13" t="s">
+      <c r="B25" s="12" t="s">
         <v>22</v>
       </c>
       <c r="E25" s="7" t="n">
         <f aca="false">E24/4</f>
-        <v>2581.62</v>
+        <v>2826.12</v>
       </c>
     </row>
     <row r="779" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>